<commit_message>
them anh + chinh sua excel
</commit_message>
<xml_diff>
--- a/data/products.xlsx
+++ b/data/products.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="99">
   <si>
     <t>STT</t>
   </si>
@@ -237,13 +237,94 @@
   </si>
   <si>
     <t>http://www.bulbs.com/product/40A15-TF-SAFETY?RefId=116</t>
+  </si>
+  <si>
+    <t>Philips 175W Clear ED17 Metal Halide Bulb</t>
+  </si>
+  <si>
+    <t>Philips</t>
+  </si>
+  <si>
+    <t>Estimated life of 9.1 years based on 3 hours use per day</t>
+  </si>
+  <si>
+    <t>Philips Lighting</t>
+  </si>
+  <si>
+    <t>MH175/U/M</t>
+  </si>
+  <si>
+    <t>175 Watts</t>
+  </si>
+  <si>
+    <t>ED-17</t>
+  </si>
+  <si>
+    <t>Cool White</t>
+  </si>
+  <si>
+    <t>Metal Halide</t>
+  </si>
+  <si>
+    <t>64479 - M175/U/M</t>
+  </si>
+  <si>
+    <t>http://www.bulbs.com/product/MH175-U-M?RefId=112</t>
+  </si>
+  <si>
+    <t>LEDlux Alsace Dimmable 3 Light Spotlight in Brushed Chrome</t>
+  </si>
+  <si>
+    <t>Lucci LEDlux</t>
+  </si>
+  <si>
+    <t>Milan Adjustable LED White Switch Spotlight in Warm White</t>
+  </si>
+  <si>
+    <t>https://www.beaconlighting.com.au/ledlux-alsace-3-light-spotlight-in-brushed-chrome.html</t>
+  </si>
+  <si>
+    <t>This fitting is for indoor use only and is not dimmable. This spot light has an on\off switch located on the facia but still needs to be installed by an electrician.</t>
+  </si>
+  <si>
+    <t>https://www.beaconlighting.com.au/milan-adjustable-led-white-switch-spotlight-in-warm-white.html</t>
+  </si>
+  <si>
+    <t>MFL</t>
+  </si>
+  <si>
+    <t>LEDlux Alsace Dimmable 1 Light Spotlight in Brushed Chrome</t>
+  </si>
+  <si>
+    <t>The LEDlux Alsace is a modern stylish dimmable spotlight that can be wall or ceiling mounted. It presents a sophisticated, low energy LED alternative to halogen spotlights. This fitting is dimmable and has been tested with the Clipsal 32E450LM, 32E450TM, 32E450UDM and LUCCI SKU 290998 dimmer.</t>
+  </si>
+  <si>
+    <t>The LEDlux Alsace is a modern stylish dimmable spotlight that can be wall or ceiling mounted. It presents a sophisticated, low energy LED alternative to halogen spotlights.This fitting is dimmable and has been tested with the Clipsal 32E450LM, 32E450TM, 32E450UDM and LUCCI SKU 290998 dimmer.</t>
+  </si>
+  <si>
+    <t>https://www.beaconlighting.com.au/ledlux-alsace-1-light-spotlight-in-brushed-chrome.html</t>
+  </si>
+  <si>
+    <t>Nevada 1 Light Track Spot in Grey</t>
+  </si>
+  <si>
+    <t>Lucci Maison</t>
+  </si>
+  <si>
+    <t>Modern with a slender design, the Nevada’s are the perfect track spot range. The Nevada track spot comes in a range colours including brushed brass, polished copper, chrome, grey and mint, white and black. This Nevada can be mounted on a ceiling and is adjustable to direct light wherever you need it and is dimmable if using a dimmable GU10 globe.</t>
+  </si>
+  <si>
+    <t>https://www.beaconlighting.com.au/nevada-1-light-track-spot-in-grey.html</t>
+  </si>
+  <si>
+    <t>LEDlux Alsace Dimmable 3 Light Spotlight in White</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -266,8 +347,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -283,6 +370,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -361,15 +454,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -380,7 +470,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -389,11 +485,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -611,6 +710,361 @@
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1352550</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>1019175</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E38427BE-4A40-4023-A275-5E8F9FA44CA6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4591050" y="4610100"/>
+          <a:ext cx="1333500" cy="1000125"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>21167</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>21166</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1344084</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>1130301</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8" descr="https://www.beaconlighting.com.au/media/catalog/product/cache/1/image/040ec09b1e35df139433887a97daa66f/1/5/150980.jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F224DE49-9A6D-4BBE-AC1C-4A7A83AC6189}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4603750" y="5672666"/>
+          <a:ext cx="1322917" cy="1109135"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>27215</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>27215</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1347107</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1749283</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10" descr="https://www.beaconlighting.com.au/media/catalog/product/cache/1/image/040ec09b1e35df139433887a97daa66f/3/0/307001.jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{720E9633-8936-4C7F-BBD7-4FB95588E84F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4599215" y="8572501"/>
+          <a:ext cx="1319892" cy="1722068"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>27214</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>27214</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1347107</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>1106065</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11" descr="https://www.beaconlighting.com.au/media/catalog/product/cache/1/image/040ec09b1e35df139433887a97daa66f/l/1/l15_alsace-v2.jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A43E27A6-8067-4F82-9751-60D91483AE77}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4599214" y="10341428"/>
+          <a:ext cx="1319893" cy="1078851"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>27215</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>27215</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>1763393</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12" descr="https://www.beaconlighting.com.au/media/catalog/product/cache/1/image/040ec09b1e35df139433887a97daa66f/1/5/159129.jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B091CDA-2D38-4019-A9EE-B12343E4EC5B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4599215" y="11742965"/>
+          <a:ext cx="1333499" cy="1736178"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>27214</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>27214</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1346435</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>1578427</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13" descr="https://www.beaconlighting.com.au/media/catalog/product/cache/1/image/040ec09b1e35df139433887a97daa66f/l/1/l16_alsace.jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E93E84ED-85D5-4DF9-B530-AB39BB34C925}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4599214" y="14382750"/>
+          <a:ext cx="1319221" cy="1551213"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -892,8 +1346,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S11" sqref="S11"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -903,7 +1357,7 @@
     <col min="4" max="4" width="16.375" customWidth="1"/>
     <col min="5" max="5" width="17.875" customWidth="1"/>
     <col min="6" max="6" width="28.75" customWidth="1"/>
-    <col min="7" max="7" width="10.5" customWidth="1"/>
+    <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.75" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="33.125" bestFit="1" customWidth="1"/>
@@ -942,868 +1396,945 @@
       <c r="F1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10"/>
-      <c r="W1" s="10"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
       <c r="X1" s="8" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="7" t="s">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K2" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="L2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="M2" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="N2" s="7" t="s">
+      <c r="N2" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="O2" s="7" t="s">
+      <c r="O2" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="P2" s="7" t="s">
+      <c r="P2" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="Q2" s="7" t="s">
+      <c r="Q2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="R2" s="7" t="s">
+      <c r="R2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="S2" s="7" t="s">
+      <c r="S2" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="T2" s="7" t="s">
+      <c r="T2" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="U2" s="7" t="s">
+      <c r="U2" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="V2" s="7" t="s">
+      <c r="V2" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="W2" s="7" t="s">
+      <c r="W2" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="X2" s="11"/>
+      <c r="X2" s="9"/>
     </row>
     <row r="3" spans="1:24" ht="81.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5">
+      <c r="A3" s="4">
         <v>1</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="6" t="s">
+      <c r="E3" s="4"/>
+      <c r="F3" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="K3" s="6">
+      <c r="K3" s="5">
         <v>120</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L3" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="M3" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="N3" s="6" t="s">
+      <c r="N3" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="O3" s="6">
+      <c r="O3" s="5">
         <v>82</v>
       </c>
-      <c r="P3" s="6">
+      <c r="P3" s="5">
         <v>2700</v>
       </c>
-      <c r="Q3" s="6" t="s">
+      <c r="Q3" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="R3" s="6" t="s">
+      <c r="R3" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="S3" s="6" t="s">
+      <c r="S3" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="T3" s="6">
+      <c r="T3" s="5">
         <v>10000</v>
       </c>
-      <c r="U3" s="6">
+      <c r="U3" s="5">
         <v>5.375</v>
       </c>
-      <c r="V3" s="6">
+      <c r="V3" s="5">
         <v>2.75</v>
       </c>
-      <c r="W3" s="6" t="s">
+      <c r="W3" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="X3" s="12" t="s">
+      <c r="X3" s="7" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:24" ht="80.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="5">
+      <c r="A4" s="4">
         <v>2</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="6" t="s">
+      <c r="E4" s="4"/>
+      <c r="F4" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="I4" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6">
+      <c r="J4" s="5"/>
+      <c r="K4" s="5">
         <v>130</v>
       </c>
-      <c r="L4" s="6" t="s">
+      <c r="L4" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="M4" s="6" t="s">
+      <c r="M4" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="N4" s="6" t="s">
+      <c r="N4" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="O4" s="6">
+      <c r="O4" s="5">
         <v>100</v>
       </c>
-      <c r="P4" s="6">
+      <c r="P4" s="5">
         <v>2700</v>
       </c>
-      <c r="Q4" s="6">
+      <c r="Q4" s="5">
         <v>560</v>
       </c>
-      <c r="R4" s="6" t="s">
+      <c r="R4" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="S4" s="6" t="s">
+      <c r="S4" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="T4" s="6">
+      <c r="T4" s="5">
         <v>5000</v>
       </c>
-      <c r="U4" s="6">
+      <c r="U4" s="5">
         <v>4.25</v>
       </c>
-      <c r="V4" s="6">
+      <c r="V4" s="5">
         <v>2.375</v>
       </c>
-      <c r="W4" s="6" t="s">
+      <c r="W4" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="X4" s="5" t="s">
+      <c r="X4" s="4" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:24" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="A5" s="5">
+      <c r="A5" s="4">
         <v>3</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="6" t="s">
+      <c r="E5" s="4"/>
+      <c r="F5" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="I5" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6">
+      <c r="J5" s="5"/>
+      <c r="K5" s="5">
         <v>120</v>
       </c>
-      <c r="L5" s="6" t="s">
+      <c r="L5" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="M5" s="6" t="s">
+      <c r="M5" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="N5" s="6" t="s">
+      <c r="N5" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="O5" s="6"/>
-      <c r="P5" s="6">
+      <c r="O5" s="5"/>
+      <c r="P5" s="5">
         <v>2000</v>
       </c>
-      <c r="Q5" s="6">
+      <c r="Q5" s="5">
         <v>200</v>
       </c>
-      <c r="R5" s="6" t="s">
+      <c r="R5" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="S5" s="6" t="s">
+      <c r="S5" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="T5" s="6">
+      <c r="T5" s="5">
         <v>3000</v>
       </c>
-      <c r="U5" s="6">
+      <c r="U5" s="5">
         <v>5.2</v>
       </c>
-      <c r="V5" s="6">
+      <c r="V5" s="5">
         <v>2.1</v>
       </c>
-      <c r="W5" s="6"/>
-      <c r="X5" s="5" t="s">
+      <c r="W5" s="5"/>
+      <c r="X5" s="4" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:24" ht="84" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="5">
+      <c r="A6" s="4">
         <v>4</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="6" t="s">
+      <c r="E6" s="4"/>
+      <c r="F6" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6" t="s">
+      <c r="H6" s="5"/>
+      <c r="I6" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6">
+      <c r="J6" s="5"/>
+      <c r="K6" s="5">
         <v>130</v>
       </c>
-      <c r="L6" s="6" t="s">
+      <c r="L6" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="M6" s="6" t="s">
+      <c r="M6" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="N6" s="6" t="s">
+      <c r="N6" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="O6" s="6">
+      <c r="O6" s="5">
         <v>100</v>
       </c>
-      <c r="P6" s="6">
+      <c r="P6" s="5">
         <v>2700</v>
       </c>
-      <c r="Q6" s="6">
+      <c r="Q6" s="5">
         <v>280</v>
       </c>
-      <c r="R6" s="6" t="s">
+      <c r="R6" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="S6" s="6" t="s">
+      <c r="S6" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="T6" s="6">
+      <c r="T6" s="5">
         <v>2500</v>
       </c>
-      <c r="U6" s="6">
+      <c r="U6" s="5">
         <v>3.5</v>
       </c>
-      <c r="V6" s="6">
+      <c r="V6" s="5">
         <v>1.9</v>
       </c>
-      <c r="W6" s="5"/>
-      <c r="X6" s="5" t="s">
+      <c r="W6" s="4"/>
+      <c r="X6" s="4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A7" s="5">
+    <row r="7" spans="1:24" ht="83.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4">
         <v>5</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5" t="s">
+      <c r="B7" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
+      <c r="D7" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>77</v>
+      </c>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
-      <c r="P7" s="5"/>
-      <c r="Q7" s="5"/>
-      <c r="R7" s="5"/>
-      <c r="S7" s="5"/>
-      <c r="T7" s="5"/>
-      <c r="U7" s="5"/>
-      <c r="V7" s="5"/>
-      <c r="W7" s="5"/>
-      <c r="X7" s="5"/>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A8" s="5">
+      <c r="L7" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="M7" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="N7" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="O7" s="5">
+        <v>65</v>
+      </c>
+      <c r="P7" s="5">
+        <v>4000</v>
+      </c>
+      <c r="Q7" s="5">
+        <v>9100</v>
+      </c>
+      <c r="R7" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="S7" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="T7" s="5">
+        <v>10000</v>
+      </c>
+      <c r="U7" s="5">
+        <v>5.44</v>
+      </c>
+      <c r="V7" s="5">
+        <v>2.125</v>
+      </c>
+      <c r="W7" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="X7" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" ht="198" x14ac:dyDescent="0.3">
+      <c r="A8" s="4">
         <v>6</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5" t="s">
+      <c r="B8" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="5"/>
-      <c r="Q8" s="5"/>
-      <c r="R8" s="5"/>
-      <c r="S8" s="5"/>
-      <c r="T8" s="5"/>
-      <c r="U8" s="5"/>
-      <c r="V8" s="5"/>
-      <c r="W8" s="5"/>
-      <c r="X8" s="5"/>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A9" s="5">
+      <c r="D8" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="13"/>
+      <c r="R8" s="4"/>
+      <c r="S8" s="4"/>
+      <c r="T8" s="4"/>
+      <c r="U8" s="4"/>
+      <c r="V8" s="4"/>
+      <c r="W8" s="4"/>
+      <c r="X8" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" ht="139.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4">
         <v>7</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5" t="s">
+      <c r="B9" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="5"/>
-      <c r="P9" s="5"/>
-      <c r="Q9" s="5"/>
-      <c r="R9" s="5"/>
-      <c r="S9" s="5"/>
-      <c r="T9" s="5"/>
-      <c r="U9" s="5"/>
-      <c r="V9" s="5"/>
-      <c r="W9" s="5"/>
-      <c r="X9" s="5"/>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A10" s="5">
+      <c r="D9" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="4"/>
+      <c r="S9" s="4"/>
+      <c r="T9" s="4"/>
+      <c r="U9" s="4"/>
+      <c r="V9" s="4"/>
+      <c r="W9" s="4"/>
+      <c r="X9" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" ht="165" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="4">
         <v>8</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5" t="s">
+      <c r="B10" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
-      <c r="P10" s="5"/>
-      <c r="Q10" s="5"/>
-      <c r="R10" s="5"/>
-      <c r="S10" s="5"/>
-      <c r="T10" s="5"/>
-      <c r="U10" s="5"/>
-      <c r="V10" s="5"/>
-      <c r="W10" s="5"/>
-      <c r="X10" s="5"/>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A11" s="5">
+      <c r="D10" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="4"/>
+      <c r="R10" s="4"/>
+      <c r="S10" s="4"/>
+      <c r="T10" s="4"/>
+      <c r="U10" s="4"/>
+      <c r="V10" s="4"/>
+      <c r="W10" s="4"/>
+      <c r="X10" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" ht="184.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4">
         <v>9</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5" t="s">
+      <c r="B11" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
-      <c r="O11" s="5"/>
-      <c r="P11" s="5"/>
-      <c r="Q11" s="5"/>
-      <c r="R11" s="5"/>
-      <c r="S11" s="5"/>
-      <c r="T11" s="5"/>
-      <c r="U11" s="5"/>
-      <c r="V11" s="5"/>
-      <c r="W11" s="5"/>
-      <c r="X11" s="5"/>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A12" s="5">
+      <c r="D11" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="4"/>
+      <c r="R11" s="4"/>
+      <c r="S11" s="4"/>
+      <c r="T11" s="4"/>
+      <c r="U11" s="4"/>
+      <c r="V11" s="4"/>
+      <c r="W11" s="4"/>
+      <c r="X11" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" ht="142.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="4">
         <v>10</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5" t="s">
+      <c r="B12" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
-      <c r="P12" s="5"/>
-      <c r="Q12" s="5"/>
-      <c r="R12" s="5"/>
-      <c r="S12" s="5"/>
-      <c r="T12" s="5"/>
-      <c r="U12" s="5"/>
-      <c r="V12" s="5"/>
-      <c r="W12" s="5"/>
-      <c r="X12" s="5"/>
+      <c r="D12" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="4"/>
+      <c r="S12" s="4"/>
+      <c r="T12" s="4"/>
+      <c r="U12" s="4"/>
+      <c r="V12" s="4"/>
+      <c r="W12" s="4"/>
+      <c r="X12" s="4"/>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A13" s="5">
+      <c r="A13" s="4">
         <v>11</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5" t="s">
+      <c r="B13" s="4"/>
+      <c r="C13" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="5"/>
-      <c r="P13" s="5"/>
-      <c r="Q13" s="5"/>
-      <c r="R13" s="5"/>
-      <c r="S13" s="5"/>
-      <c r="T13" s="5"/>
-      <c r="U13" s="5"/>
-      <c r="V13" s="5"/>
-      <c r="W13" s="5"/>
-      <c r="X13" s="5"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
+      <c r="R13" s="4"/>
+      <c r="S13" s="4"/>
+      <c r="T13" s="4"/>
+      <c r="U13" s="4"/>
+      <c r="V13" s="4"/>
+      <c r="W13" s="4"/>
+      <c r="X13" s="4"/>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A14" s="5">
+      <c r="A14" s="4">
         <v>12</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5" t="s">
+      <c r="B14" s="4"/>
+      <c r="C14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="5"/>
-      <c r="P14" s="5"/>
-      <c r="Q14" s="5"/>
-      <c r="R14" s="5"/>
-      <c r="S14" s="5"/>
-      <c r="T14" s="5"/>
-      <c r="U14" s="5"/>
-      <c r="V14" s="5"/>
-      <c r="W14" s="5"/>
-      <c r="X14" s="5"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="4"/>
+      <c r="R14" s="4"/>
+      <c r="S14" s="4"/>
+      <c r="T14" s="4"/>
+      <c r="U14" s="4"/>
+      <c r="V14" s="4"/>
+      <c r="W14" s="4"/>
+      <c r="X14" s="4"/>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A15" s="5">
+      <c r="A15" s="4">
         <v>13</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5" t="s">
+      <c r="B15" s="4"/>
+      <c r="C15" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
-      <c r="N15" s="5"/>
-      <c r="O15" s="5"/>
-      <c r="P15" s="5"/>
-      <c r="Q15" s="5"/>
-      <c r="R15" s="5"/>
-      <c r="S15" s="5"/>
-      <c r="T15" s="5"/>
-      <c r="U15" s="5"/>
-      <c r="V15" s="5"/>
-      <c r="W15" s="5"/>
-      <c r="X15" s="5"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="4"/>
+      <c r="P15" s="4"/>
+      <c r="Q15" s="4"/>
+      <c r="R15" s="4"/>
+      <c r="S15" s="4"/>
+      <c r="T15" s="4"/>
+      <c r="U15" s="4"/>
+      <c r="V15" s="4"/>
+      <c r="W15" s="4"/>
+      <c r="X15" s="4"/>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A16" s="5">
+      <c r="A16" s="4">
         <v>14</v>
       </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5" t="s">
+      <c r="B16" s="4"/>
+      <c r="C16" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
-      <c r="N16" s="5"/>
-      <c r="O16" s="5"/>
-      <c r="P16" s="5"/>
-      <c r="Q16" s="5"/>
-      <c r="R16" s="5"/>
-      <c r="S16" s="5"/>
-      <c r="T16" s="5"/>
-      <c r="U16" s="5"/>
-      <c r="V16" s="5"/>
-      <c r="W16" s="5"/>
-      <c r="X16" s="5"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="4"/>
+      <c r="Q16" s="4"/>
+      <c r="R16" s="4"/>
+      <c r="S16" s="4"/>
+      <c r="T16" s="4"/>
+      <c r="U16" s="4"/>
+      <c r="V16" s="4"/>
+      <c r="W16" s="4"/>
+      <c r="X16" s="4"/>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A17" s="5">
+      <c r="A17" s="4">
         <v>15</v>
       </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5" t="s">
+      <c r="B17" s="4"/>
+      <c r="C17" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
-      <c r="O17" s="5"/>
-      <c r="P17" s="5"/>
-      <c r="Q17" s="5"/>
-      <c r="R17" s="5"/>
-      <c r="S17" s="5"/>
-      <c r="T17" s="5"/>
-      <c r="U17" s="5"/>
-      <c r="V17" s="5"/>
-      <c r="W17" s="5"/>
-      <c r="X17" s="5"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="4"/>
+      <c r="Q17" s="4"/>
+      <c r="R17" s="4"/>
+      <c r="S17" s="4"/>
+      <c r="T17" s="4"/>
+      <c r="U17" s="4"/>
+      <c r="V17" s="4"/>
+      <c r="W17" s="4"/>
+      <c r="X17" s="4"/>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A18" s="5">
+      <c r="A18" s="4">
         <v>16</v>
       </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5" t="s">
+      <c r="B18" s="4"/>
+      <c r="C18" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
-      <c r="O18" s="5"/>
-      <c r="P18" s="5"/>
-      <c r="Q18" s="5"/>
-      <c r="R18" s="5"/>
-      <c r="S18" s="5"/>
-      <c r="T18" s="5"/>
-      <c r="U18" s="5"/>
-      <c r="V18" s="5"/>
-      <c r="W18" s="5"/>
-      <c r="X18" s="5"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+      <c r="P18" s="4"/>
+      <c r="Q18" s="4"/>
+      <c r="R18" s="4"/>
+      <c r="S18" s="4"/>
+      <c r="T18" s="4"/>
+      <c r="U18" s="4"/>
+      <c r="V18" s="4"/>
+      <c r="W18" s="4"/>
+      <c r="X18" s="4"/>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A19" s="5">
+      <c r="A19" s="4">
         <v>17</v>
       </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5" t="s">
+      <c r="B19" s="4"/>
+      <c r="C19" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="5"/>
-      <c r="N19" s="5"/>
-      <c r="O19" s="5"/>
-      <c r="P19" s="5"/>
-      <c r="Q19" s="5"/>
-      <c r="R19" s="5"/>
-      <c r="S19" s="5"/>
-      <c r="T19" s="5"/>
-      <c r="U19" s="5"/>
-      <c r="V19" s="5"/>
-      <c r="W19" s="5"/>
-      <c r="X19" s="5"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="4"/>
+      <c r="Q19" s="4"/>
+      <c r="R19" s="4"/>
+      <c r="S19" s="4"/>
+      <c r="T19" s="4"/>
+      <c r="U19" s="4"/>
+      <c r="V19" s="4"/>
+      <c r="W19" s="4"/>
+      <c r="X19" s="4"/>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A20" s="5">
+      <c r="A20" s="4">
         <v>18</v>
       </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5" t="s">
+      <c r="B20" s="4"/>
+      <c r="C20" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
-      <c r="N20" s="5"/>
-      <c r="O20" s="5"/>
-      <c r="P20" s="5"/>
-      <c r="Q20" s="5"/>
-      <c r="R20" s="5"/>
-      <c r="S20" s="5"/>
-      <c r="T20" s="5"/>
-      <c r="U20" s="5"/>
-      <c r="V20" s="5"/>
-      <c r="W20" s="5"/>
-      <c r="X20" s="5"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="4"/>
+      <c r="Q20" s="4"/>
+      <c r="R20" s="4"/>
+      <c r="S20" s="4"/>
+      <c r="T20" s="4"/>
+      <c r="U20" s="4"/>
+      <c r="V20" s="4"/>
+      <c r="W20" s="4"/>
+      <c r="X20" s="4"/>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A21" s="5">
+      <c r="A21" s="4">
         <v>19</v>
       </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5" t="s">
+      <c r="B21" s="4"/>
+      <c r="C21" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="5"/>
-      <c r="N21" s="5"/>
-      <c r="O21" s="5"/>
-      <c r="P21" s="5"/>
-      <c r="Q21" s="5"/>
-      <c r="R21" s="5"/>
-      <c r="S21" s="5"/>
-      <c r="T21" s="5"/>
-      <c r="U21" s="5"/>
-      <c r="V21" s="5"/>
-      <c r="W21" s="5"/>
-      <c r="X21" s="5"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+      <c r="O21" s="4"/>
+      <c r="P21" s="4"/>
+      <c r="Q21" s="4"/>
+      <c r="R21" s="4"/>
+      <c r="S21" s="4"/>
+      <c r="T21" s="4"/>
+      <c r="U21" s="4"/>
+      <c r="V21" s="4"/>
+      <c r="W21" s="4"/>
+      <c r="X21" s="4"/>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A22" s="5">
+      <c r="A22" s="4">
         <v>20</v>
       </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5" t="s">
+      <c r="B22" s="4"/>
+      <c r="C22" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
-      <c r="M22" s="5"/>
-      <c r="N22" s="5"/>
-      <c r="O22" s="5"/>
-      <c r="P22" s="5"/>
-      <c r="Q22" s="5"/>
-      <c r="R22" s="5"/>
-      <c r="S22" s="5"/>
-      <c r="T22" s="5"/>
-      <c r="U22" s="5"/>
-      <c r="V22" s="5"/>
-      <c r="W22" s="5"/>
-      <c r="X22" s="5"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+      <c r="O22" s="4"/>
+      <c r="P22" s="4"/>
+      <c r="Q22" s="4"/>
+      <c r="R22" s="4"/>
+      <c r="S22" s="4"/>
+      <c r="T22" s="4"/>
+      <c r="U22" s="4"/>
+      <c r="V22" s="4"/>
+      <c r="W22" s="4"/>
+      <c r="X22" s="4"/>
     </row>
     <row r="23" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="5"/>
-      <c r="L23" s="5"/>
-      <c r="M23" s="5"/>
-      <c r="N23" s="5"/>
-      <c r="O23" s="5"/>
-      <c r="P23" s="5"/>
-      <c r="Q23" s="5"/>
-      <c r="R23" s="5"/>
-      <c r="S23" s="5"/>
-      <c r="T23" s="5"/>
-      <c r="U23" s="5"/>
-      <c r="V23" s="5"/>
-      <c r="W23" s="5"/>
-      <c r="X23" s="5"/>
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
+      <c r="N23" s="4"/>
+      <c r="O23" s="4"/>
+      <c r="P23" s="4"/>
+      <c r="Q23" s="4"/>
+      <c r="R23" s="4"/>
+      <c r="S23" s="4"/>
+      <c r="T23" s="4"/>
+      <c r="U23" s="4"/>
+      <c r="V23" s="4"/>
+      <c r="W23" s="4"/>
+      <c r="X23" s="4"/>
     </row>
     <row r="24" spans="1:24" s="3" customFormat="1" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
@@ -1836,14 +2367,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:W1"/>
+    <mergeCell ref="X1:X2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:W1"/>
-    <mergeCell ref="X1:X2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="X3" r:id="rId1"/>
@@ -1924,13 +2455,13 @@
       <c r="E5" s="1"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>